<commit_message>
implementando o cadastro do usuário
</commit_message>
<xml_diff>
--- a/docs/Cronograma de Atividades.xlsx
+++ b/docs/Cronograma de Atividades.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$I$17</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -343,7 +346,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,10 +395,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,10 +432,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,30 +511,34 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
+      <selection pane="bottomLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.87244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.1071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="32.2448979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="2.31122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.17857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.219387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,7 +587,7 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -609,7 +608,7 @@
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -631,17 +630,16 @@
         <v>18</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="6" t="s">
         <v>17</v>
       </c>
@@ -649,9 +647,8 @@
         <v>20</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
         <v>21</v>
@@ -660,10 +657,10 @@
         <v>22</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
@@ -672,7 +669,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
       <c r="B7" s="10" t="s">
         <v>26</v>
@@ -681,7 +678,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="11" t="n">
@@ -694,9 +691,8 @@
         <v>27</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
         <v>28</v>
@@ -705,10 +701,10 @@
         <v>26</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
@@ -717,7 +713,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>26</v>
@@ -726,10 +722,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="6" t="s">
         <v>24</v>
       </c>
@@ -738,25 +734,25 @@
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" s="18" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
+    <row r="10" s="17" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="11" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="6"/>
@@ -773,15 +769,15 @@
         <v>32</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -792,7 +788,7 @@
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="13" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
         <v>21</v>
@@ -815,12 +811,12 @@
       </c>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="11"/>
@@ -832,7 +828,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="15" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
         <v>21</v>
@@ -841,7 +837,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="11"/>
@@ -853,12 +849,12 @@
       </c>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="16" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="11"/>
@@ -870,332 +866,219 @@
       </c>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" s="18" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="17" t="s">
+    <row r="17" s="17" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="10"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="6"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A19" s="6"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="9"/>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="I20" s="9"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="22"/>
+      <c r="B21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="9"/>
+      <c r="B22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="9"/>
+      <c r="E23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="24" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="9"/>
+      <c r="E24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="25" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A27" s="6"/>
+    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22"/>
+      <c r="B26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="22"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I29" s="17"/>
-    </row>
-    <row r="30" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="23"/>
-      <c r="J31" s="12"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A32" s="6"/>
-      <c r="B32" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="11" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A34" s="6"/>
-      <c r="B34" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="11" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A36" s="24"/>
-      <c r="B36" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I36" s="21"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A37" s="24"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I37" s="21"/>
-    </row>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:I17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1203,5 +1086,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
versionando os assets enviados por Tuca
</commit_message>
<xml_diff>
--- a/docs/Cronograma de Atividades.xlsx
+++ b/docs/Cronograma de Atividades.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$I$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$I$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$I$19</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -96,12 +97,24 @@
     <t xml:space="preserve">16/11/2016</t>
   </si>
   <si>
+    <t xml:space="preserve">Concluído</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time</t>
   </si>
   <si>
     <t xml:space="preserve">Definir APP do Cliente com TUCA</t>
   </si>
   <si>
+    <t xml:space="preserve">17/11/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/11/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviar assets para Arthur e Roberto</t>
+  </si>
+  <si>
     <t xml:space="preserve">A Fazer</t>
   </si>
   <si>
@@ -114,9 +127,6 @@
     <t xml:space="preserve">01/11/2016</t>
   </si>
   <si>
-    <t xml:space="preserve">Concluído</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gilberto</t>
   </si>
   <si>
@@ -135,10 +145,19 @@
     <t xml:space="preserve">Ajustar a API para retornar código de erro</t>
   </si>
   <si>
+    <t xml:space="preserve">22/11/2016</t>
+  </si>
+  <si>
     <t xml:space="preserve">API de revogação de Token: Logout</t>
   </si>
   <si>
+    <t xml:space="preserve">Implementar API: demonstrar interesse do profissional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Versão WEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/11/2016</t>
   </si>
   <si>
     <t xml:space="preserve">Cadastro Usuário: Cadastro básico funcional</t>
@@ -254,14 +273,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF009900"/>
+      <color rgb="FFDD4814"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFDD4814"/>
+      <color rgb="FF009900"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -346,7 +365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -391,11 +410,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,16 +438,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -522,23 +545,22 @@
   </sheetPr>
   <dimension ref="A1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.219387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.41836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="35.8163265306122"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="2.34183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,7 +630,7 @@
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -617,235 +639,243 @@
         <v>16</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="F4" s="11" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="6"/>
       <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6"/>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="11" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="13" t="s">
+      <c r="H8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" s="17" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="13"/>
+      <c r="G10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
-      <c r="B11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>16</v>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="11" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="E11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="13"/>
       <c r="G11" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" s="17" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="11" t="n">
-        <v>0.1</v>
+      <c r="F13" s="12" t="n">
+        <v>0.9</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I13" s="9"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="11"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="G14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="11"/>
+      <c r="E15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="12" t="n">
+        <v>0.1</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -854,43 +884,57 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="11"/>
+      <c r="E16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="12"/>
       <c r="G16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" s="17" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="F18" s="12"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="9"/>
+      <c r="G18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="17" customFormat="true" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -899,176 +943,200 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="16" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
-      <c r="B20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
-      <c r="B21" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>
-      <c r="B22" s="10" t="s">
-        <v>26</v>
+      <c r="B22" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="11" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="20" t="n">
+        <v>0.9</v>
+      </c>
       <c r="G23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="21" t="n">
+        <v>0.8</v>
+      </c>
       <c r="G24" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6"/>
+      <c r="B26" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="11" t="n">
+      <c r="F27" s="21" t="n">
         <v>0.9</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22"/>
-      <c r="B26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="9" t="s">
+      <c r="G27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="6"/>
       <c r="H27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>38</v>
+      </c>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="23"/>
+      <c r="B28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="23"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="19"/>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1078,7 +1146,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:I17"/>
+  <autoFilter ref="A1:I19"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>